<commit_message>
added top 10 citites seperate endpoint
</commit_message>
<xml_diff>
--- a/DISTRICT_WISE_CENSUS_RESULTS_CENSUS_2017.xlsx
+++ b/DISTRICT_WISE_CENSUS_RESULTS_CENSUS_2017.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="440" windowWidth="33600" windowHeight="18900" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="440" windowWidth="33600" windowHeight="18900" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Raw" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="888" uniqueCount="758">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="888" uniqueCount="768">
   <si>
     <t>TABLE - 1: PROVISIONAL PROVINCE WISE POPULATION BY SEX AND RURAL/URBAN</t>
   </si>
@@ -2304,6 +2304,36 @@
   </si>
   <si>
     <t>City</t>
+  </si>
+  <si>
+    <t>Karachi</t>
+  </si>
+  <si>
+    <t>Lahore</t>
+  </si>
+  <si>
+    <t>Faislabad</t>
+  </si>
+  <si>
+    <t>Rawalpindi</t>
+  </si>
+  <si>
+    <t>Gujranwala</t>
+  </si>
+  <si>
+    <t>Peshawar</t>
+  </si>
+  <si>
+    <t>Multan</t>
+  </si>
+  <si>
+    <t>Hyderabad</t>
+  </si>
+  <si>
+    <t>Islamabad</t>
+  </si>
+  <si>
+    <t>Quetta</t>
   </si>
 </sst>
 </file>
@@ -3014,7 +3044,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:I684"/>
   <sheetViews>
-    <sheetView topLeftCell="A650" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A671" sqref="A671:C684"/>
     </sheetView>
   </sheetViews>
@@ -19165,8 +19195,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -19188,7 +19218,7 @@
     </row>
     <row r="2" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>741</v>
+        <v>758</v>
       </c>
       <c r="B2" s="21">
         <v>14910352</v>
@@ -19199,7 +19229,7 @@
     </row>
     <row r="3" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>742</v>
+        <v>759</v>
       </c>
       <c r="B3" s="21">
         <v>11126285</v>
@@ -19210,7 +19240,7 @@
     </row>
     <row r="4" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>743</v>
+        <v>760</v>
       </c>
       <c r="B4" s="21">
         <v>3203846</v>
@@ -19221,7 +19251,7 @@
     </row>
     <row r="5" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>744</v>
+        <v>761</v>
       </c>
       <c r="B5" s="21">
         <v>2098231</v>
@@ -19232,7 +19262,7 @@
     </row>
     <row r="6" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>745</v>
+        <v>762</v>
       </c>
       <c r="B6" s="21">
         <v>2027001</v>
@@ -19243,7 +19273,7 @@
     </row>
     <row r="7" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>746</v>
+        <v>763</v>
       </c>
       <c r="B7" s="21">
         <v>1970042</v>
@@ -19254,7 +19284,7 @@
     </row>
     <row r="8" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>747</v>
+        <v>764</v>
       </c>
       <c r="B8" s="21">
         <v>1871843</v>
@@ -19265,7 +19295,7 @@
     </row>
     <row r="9" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>748</v>
+        <v>765</v>
       </c>
       <c r="B9" s="21">
         <v>1732693</v>
@@ -19276,7 +19306,7 @@
     </row>
     <row r="10" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>749</v>
+        <v>766</v>
       </c>
       <c r="B10" s="21">
         <v>1014825</v>
@@ -19287,7 +19317,7 @@
     </row>
     <row r="11" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>750</v>
+        <v>767</v>
       </c>
       <c r="B11" s="21">
         <v>1001205</v>
@@ -19308,8 +19338,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G44" sqref="G44"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -19541,7 +19571,7 @@
   <dimension ref="A1:J100"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>

</xml_diff>